<commit_message>
add and fix function Exam group sub question
</commit_message>
<xml_diff>
--- a/GROUP01_Exel.xlsx
+++ b/GROUP01_Exel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -90,51 +90,6 @@
   </si>
   <si>
     <t>lam@gmail.com</t>
-  </si>
-  <si>
-    <t>S005</t>
-  </si>
-  <si>
-    <t>Mai Ánh</t>
-  </si>
-  <si>
-    <t>Tuyết</t>
-  </si>
-  <si>
-    <t>0988888880</t>
-  </si>
-  <si>
-    <t>tuyet@gmail.com</t>
-  </si>
-  <si>
-    <t>S006</t>
-  </si>
-  <si>
-    <t>Lê Thị Bích</t>
-  </si>
-  <si>
-    <t>Tuyền</t>
-  </si>
-  <si>
-    <t>0399999999</t>
-  </si>
-  <si>
-    <t>tuyen@gmail.com</t>
-  </si>
-  <si>
-    <t>S007</t>
-  </si>
-  <si>
-    <t>Nguyễn Thu</t>
-  </si>
-  <si>
-    <t>Minh</t>
-  </si>
-  <si>
-    <t>0395555555</t>
-  </si>
-  <si>
-    <t>minh@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -199,7 +154,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -209,7 +164,7 @@
     <col min="2" max="2" width="14.25" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.97265625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="10.9296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.609375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.87109375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="9.6484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -301,57 +256,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>